<commit_message>
Add stage3 evidence / B1-B2
</commit_message>
<xml_diff>
--- a/timveltman3/evidence.xlsx
+++ b/timveltman3/evidence.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\timveltman3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\0k_timveltman3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4AE1E02-5209-4D23-9477-D7E58B499BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7A19F5-7FD6-4DA6-9B4D-172DFCB1CD30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="889" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="43">
   <si>
     <t>TxHash</t>
   </si>
@@ -161,6 +161,18 @@
   </si>
   <si>
     <t>ibc/A45852C0C4404F1C85EB484CF3CC227AFFDE0340CF4450398A78CB48DC7F002D</t>
+  </si>
+  <si>
+    <t>A8714DADFE7C5F64101B198DBFE466FCDDD277C15CBDAE7A36548C325EAD6CD9</t>
+  </si>
+  <si>
+    <t>B0CA2688210CB1120BBFB2A020C3FCA4FC715E8707C1457C8349008441919B6F</t>
+  </si>
+  <si>
+    <t>7B762579D847876E32D782EB4456C813AB8EFE1F224B34FDB40F8A4F00FA56EC</t>
+  </si>
+  <si>
+    <t>1BC72E7F6FAAA96374C241AD88A674C26FEE6ECDE15A454319AB75B764F783FA</t>
   </si>
 </sst>
 </file>
@@ -557,8 +569,8 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1200,7 +1212,9 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1214,12 +1228,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1234,7 +1248,9 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1248,12 +1264,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add stage2 evidence / A7-A20
</commit_message>
<xml_diff>
--- a/timveltman3/evidence.xlsx
+++ b/timveltman3/evidence.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\0k_timveltman3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\_0k_timveltman3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7A19F5-7FD6-4DA6-9B4D-172DFCB1CD30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243126E8-C06C-4C3B-8E8C-63EFCB61369F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="889" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="89">
   <si>
     <t>TxHash</t>
   </si>
@@ -58,27 +58,12 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>ClassID</t>
   </si>
   <si>
     <t>NFTID</t>
   </si>
   <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>nft id</t>
-  </si>
-  <si>
     <t>TeamName</t>
   </si>
   <si>
@@ -173,13 +158,166 @@
   </si>
   <si>
     <t>1BC72E7F6FAAA96374C241AD88A674C26FEE6ECDE15A454319AB75B764F783FA</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>ibc/207224123858AC5201C7F19181ED600FF5A66ADC52082414C8B8ED0507568B01</t>
+  </si>
+  <si>
+    <t>timveltmanA7Flowa1</t>
+  </si>
+  <si>
+    <t>ibc/A12019D5F83A9118D1FFDB4420A4D1F0C191036E85448163D60C11A16726BA31</t>
+  </si>
+  <si>
+    <t>timveltmanA9Flowa3</t>
+  </si>
+  <si>
+    <t>timveltmanA9Flowa2</t>
+  </si>
+  <si>
+    <t>ibc/F087E6C7094843F25E5911A5E6C0C13F0AB6137051AE8BDA472709A58E4578A2</t>
+  </si>
+  <si>
+    <t>ibc/A694536ECC85B6CD0D1597F44D593AC083FA591D581EECAA08E9FE5C9A773C2F</t>
+  </si>
+  <si>
+    <t>timveltmanA10Flowa4</t>
+  </si>
+  <si>
+    <t>ibc/EEFEE70B57856B298DD0B9EFA10D47CE11FF0CA0FA654CE34EBD18939F6145DF</t>
+  </si>
+  <si>
+    <t>timveltmanA11Flowa5</t>
+  </si>
+  <si>
+    <t>timveltmanA12Flowa6</t>
+  </si>
+  <si>
+    <t>ibc/D9A52EED16D188981EF86210645BF36BAFFC615C27706634001D00EC29DF52FC</t>
+  </si>
+  <si>
+    <t>3ECBD741C3993D8AF04318CE7140542D256B4288FB11A1482E9737CD75F19E73</t>
+  </si>
+  <si>
+    <t>7AF9AF49436EA16EF42DFBBE1E1B38FABE03394F104E868DA213CCDE20F27BB9</t>
+  </si>
+  <si>
+    <t>AD2B5322FD42C535368A4CD96C2256938FB73A30E12B6DEAB155A4717D70926C</t>
+  </si>
+  <si>
+    <t>7ADC50960F7EA832D33D86D73708AE467E32D1795B43B74725CD717767FB22E0</t>
+  </si>
+  <si>
+    <t>117D2BB16479F86B7EE02980DB89E50BBB34EB27C84D87E6D83B271E37FE1305</t>
+  </si>
+  <si>
+    <t>EC7CCD9663AA5E11523D8678AAC3E0F566EF61806C748C00E5C76766DD36FFA7</t>
+  </si>
+  <si>
+    <t>8F0E97F2907DAC54FC0A08481C07A57387421B5EFBE3EA93E2B080F9F537FD7B</t>
+  </si>
+  <si>
+    <t>A013580CEE7BDBD51B62F1BFBCF62291848B71A689A381CCAB39CCA3EF780775</t>
+  </si>
+  <si>
+    <t>C5DF8E81DB535B05F994CE8C78692336AA52110EF4A67060E829E0ABBC5BCFD2</t>
+  </si>
+  <si>
+    <t>6BC5BEC46A060570BBAEFCAAEDD8E8BFBBE025C9C4A298C75560E76AF66F7F4E</t>
+  </si>
+  <si>
+    <t>1C603C6B089B192B13B38F78CF790B2B788D0CFA85D3AD9E79D946BE6388C208</t>
+  </si>
+  <si>
+    <t>A06F9AF4DC8E6203C7E7F5B5E53E9C2F10384F941C2792E28AC51B115104954E</t>
+  </si>
+  <si>
+    <t>E975CEAC54B8DAB89CEA4418531386A0C6BEE8E3D9B461024593D34250034CE8</t>
+  </si>
+  <si>
+    <t>FC43EB0853A15898020E339541569527972B51BB2AB9FA0C1AEA636B98908B3D</t>
+  </si>
+  <si>
+    <t>F84E7CB3DC1EF8FCFFC303B993A0C99BFA980B32F45884B809C9A8175321C153</t>
+  </si>
+  <si>
+    <t>09798F16316D25C3D094B47B84629538711EB81010AD96F9A3A69C475F155C47</t>
+  </si>
+  <si>
+    <t>5B3ED90EF0BA08EB3109F9FAB8B95C029FD96F04CB31FE25050478FF1B7DC098</t>
+  </si>
+  <si>
+    <t>522093191D593F4E5926B0F3CDA97DCCD5D6DB97079999165016C877B5D18E74</t>
+  </si>
+  <si>
+    <t>61768D125CFD7210F90744DF9CAB2D8A8EF0B02DEE6F48304B4AF6F759B33CBB</t>
+  </si>
+  <si>
+    <t>5211DD93300ABBD9AACF80A847A9158AC29EA72011E127F750FC9A004656A790</t>
+  </si>
+  <si>
+    <t>6069154B27623DEE05BA71850377F84662126B313FC4707CF147873383EA5149</t>
+  </si>
+  <si>
+    <t>D2CC1E9DEDF399B667ED17C30BB19100DED6BBBA62D36960D4E6C95C6AB46B86</t>
+  </si>
+  <si>
+    <t>59FA9225D147CAA98454BAC7887E924E50BEC02BF63BFEFA54030959F82865D7</t>
+  </si>
+  <si>
+    <t>911AFF84CBFB0AB5885194BE41EF67B97643199F12B07940D4E1C5540805FCA5</t>
+  </si>
+  <si>
+    <t>D9C6DDC092948003F060B2A84BE2372E4C5E60D61234D53B8619A764649D3DDE</t>
+  </si>
+  <si>
+    <t>8E40FA85FD3C0EDE4C5C9BFC55184A54255955258C6D4663FCC3BBF1F92D45BC</t>
+  </si>
+  <si>
+    <t>862F9A0C049092BFF83467C9393A40686E37F466B58F453EF82D751D18A95A3C</t>
+  </si>
+  <si>
+    <t>B8F1711A7A83D4092D3FC34D4593181379384385689A5AB04E37A810AA77DFAD</t>
+  </si>
+  <si>
+    <t>8472F0B76982E9E41AFDADBAD5D5C09E085235ADAD08BB1BD8F39A2BF620E55E</t>
+  </si>
+  <si>
+    <t>D87AA066244E2CACB792502BBAC62D2F578CE53540450B0FD54670BB5E776363</t>
+  </si>
+  <si>
+    <t>28D022DD25C5F0A30906B9A93442D9FBDCEBF95B9BE9FA8775374D94A631A3EB</t>
+  </si>
+  <si>
+    <t>1989EFEEA51730205498547132B0EA0E954D8E039D45E5506C3FBCE550098033</t>
+  </si>
+  <si>
+    <t>26D0E94E12187853871EE3C208ECF06442756F77965583C6DDEDA0E67B3B6F94</t>
+  </si>
+  <si>
+    <t>5A344FE6BF90A5CBD670FA4468B7C63BDECFEC3612BBFC6AA97718A22EEEFF3C</t>
+  </si>
+  <si>
+    <t>913EE3A847A2026D52B5662195B4B504F84D760CF69DC36B81989166D05F9132</t>
+  </si>
+  <si>
+    <t>C4D61F688B3B277A3A079855741DFFF3C1E7E72B54D1329CF6E7825B167FCF11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,6 +330,19 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -243,10 +394,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -262,9 +422,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="2" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="10">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 10" xfId="9" xr:uid="{E99013DF-B514-4BED-9F0E-7D39AB9BD543}"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{73A929D9-ED37-46DA-A38B-281778BF551F}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{72671EE4-5C3C-4671-9CEE-649BFFCDD4B2}"/>
+    <cellStyle name="Normal 4" xfId="3" xr:uid="{FFFB3818-34F8-4211-B673-69F9C5561AC6}"/>
+    <cellStyle name="Normal 5" xfId="4" xr:uid="{F60EB366-B003-4DFE-B65A-E5644407F032}"/>
+    <cellStyle name="Normal 6" xfId="5" xr:uid="{09176CFE-C562-4A03-80CC-9EC16CE0C391}"/>
+    <cellStyle name="Normal 7" xfId="6" xr:uid="{5AAD6102-00F3-4CE3-9CD6-F2F466D7B133}"/>
+    <cellStyle name="Normal 8" xfId="7" xr:uid="{EBBBBC5A-0352-4EE4-8F9A-10573B210AD0}"/>
+    <cellStyle name="Normal 9" xfId="8" xr:uid="{60AE94B9-7938-4630-A2F4-558F8414AD25}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -587,51 +804,51 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="H2" s="4"/>
     </row>
@@ -647,7 +864,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -657,18 +876,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -683,7 +902,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -693,18 +914,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -719,7 +940,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -729,18 +952,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -755,7 +978,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -765,18 +990,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -789,9 +1014,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -808,24 +1035,36 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
+      <c r="A2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+      <c r="A3" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+      <c r="A4" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -837,9 +1076,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -856,24 +1097,36 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
+      <c r="A2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+      <c r="A3" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+      <c r="A4" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -885,9 +1138,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -904,24 +1159,36 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
+      <c r="A2" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+      <c r="A3" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+      <c r="A4" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -933,9 +1200,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -952,24 +1221,36 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
+      <c r="A2" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+      <c r="A3" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+      <c r="A4" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -981,9 +1262,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1000,24 +1283,36 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
+      <c r="A2" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+      <c r="A3" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+      <c r="A4" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1029,9 +1324,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1048,24 +1345,36 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
+      <c r="A2" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+      <c r="A3" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+      <c r="A4" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1093,15 +1402,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1114,9 +1423,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1133,24 +1444,52 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
+      <c r="A2" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+      <c r="A3" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+      <c r="A4" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1162,9 +1501,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1181,24 +1522,52 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
+      <c r="A2" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+      <c r="A3" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+      <c r="A4" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1228,12 +1597,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1249,7 +1618,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1264,12 +1633,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1367,32 +1736,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1423,10 +1792,112 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1437,115 +1908,13 @@
         <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1577,10 +1946,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1588,16 +1957,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1612,7 +1981,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1622,18 +1993,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1648,7 +2019,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1658,18 +2031,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add evidence / B5-B6-B7
</commit_message>
<xml_diff>
--- a/timveltman3/evidence.xlsx
+++ b/timveltman3/evidence.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
-  <workbookPr/>
+  <workbookPr codeName="BuÇalışmaKitabı"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\_0k_timveltman3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\_ALL_timveltman3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243126E8-C06C-4C3B-8E8C-63EFCB61369F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEAAE728-F0EF-4CDF-892B-6970B135CD35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="889" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="889" firstSheet="3" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,23 +38,18 @@
     <sheet name="B2" sheetId="23" r:id="rId23"/>
     <sheet name="B5" sheetId="24" r:id="rId24"/>
     <sheet name="B6" sheetId="25" r:id="rId25"/>
+    <sheet name="B7" sheetId="26" r:id="rId26"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="93">
   <si>
     <t>TxHash</t>
   </si>
   <si>
-    <t>The first Interchain NFT-Transfer TxHash</t>
-  </si>
-  <si>
-    <t>The Internal Transfer TxHash on IRISnet</t>
-  </si>
-  <si>
     <t>ChainID</t>
   </si>
   <si>
@@ -311,6 +306,24 @@
   </si>
   <si>
     <t>C4D61F688B3B277A3A079855741DFFF3C1E7E72B54D1329CF6E7825B167FCF11</t>
+  </si>
+  <si>
+    <t>D77490C37EE08F84586E86AB3AEF2FAD7553319241DFBA737D5695DB2FAA4C9B</t>
+  </si>
+  <si>
+    <t>542D43D96E684E854336E6BF43829885A41299C51337FBCA5CDF5F5D31DF58F3</t>
+  </si>
+  <si>
+    <t>0C9F6DCB44A39B768C5A3B657BCB65B42D45654D37B0F845E758A454C4647C79</t>
+  </si>
+  <si>
+    <t>73E9AA6713D6740EA14223D7AA2BF264363916FCB40E3D9D5FB34266CCF18F58</t>
+  </si>
+  <si>
+    <t>E625C66154CF858E2B1E2EA893823ED820E890D36F05793A4D0CD6E2D27E352C</t>
+  </si>
+  <si>
+    <t>3CDF8E7847A532CDCD02796D29FBEAEB0972A4317F0B4234DBF4BAFB847BFD11</t>
   </si>
 </sst>
 </file>
@@ -781,7 +794,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Sayfa1">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:H2"/>
@@ -804,51 +817,51 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="E2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="H2" s="4"/>
     </row>
@@ -859,7 +872,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Sayfa10">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
@@ -876,18 +889,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -897,7 +910,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Sayfa11">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
@@ -914,10 +927,48 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <sheetPr codeName="Sayfa12">
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -933,15 +984,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <sheetPr>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <sheetPr codeName="Sayfa13">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,34 +1003,34 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <sheetPr codeName="Sayfa14">
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -990,34 +1041,405 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <sheetPr codeName="Sayfa15">
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <sheetPr codeName="Sayfa16">
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <sheetPr codeName="Sayfa17">
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <sheetPr codeName="Sayfa18">
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <sheetPr codeName="Sayfa19">
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sayfa2">
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <sheetPr codeName="Sayfa20">
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,55 +1453,71 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <c r="A5" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+  <sheetPr codeName="Sayfa21">
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,480 +1531,55 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1576,7 +1589,7 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Sayfa22">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:A3"/>
@@ -1596,6 +1609,42 @@
       </c>
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+  <sheetPr codeName="Sayfa23">
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>34</v>
       </c>
@@ -1610,15 +1659,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
-  <sheetPr>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+  <sheetPr codeName="Sayfa24">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1633,27 +1682,29 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
-  <sheetPr>
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+  <sheetPr codeName="Sayfa25">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1667,31 +1718,30 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82F8190A-66EB-47D4-8234-87082D07AFC0}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1701,12 +1751,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1716,7 +1766,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Sayfa3">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:C3"/>
@@ -1736,32 +1786,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1771,7 +1821,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Sayfa4">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:D2"/>
@@ -1792,27 +1842,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1822,7 +1872,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Sayfa5">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:D2"/>
@@ -1843,27 +1893,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1873,7 +1923,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Sayfa6">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:D2"/>
@@ -1894,27 +1944,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1924,7 +1974,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Sayfa7">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:D2"/>
@@ -1946,27 +1996,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1976,7 +2026,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Sayfa8">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
@@ -1993,18 +2043,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -2014,7 +2064,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Sayfa9">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
@@ -2031,18 +2081,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>